<commit_message>
Push working hash and finished getGrammar()
</commit_message>
<xml_diff>
--- a/LangSpecs/First and Follow Sets.xlsx
+++ b/LangSpecs/First and Follow Sets.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/CodingProjects/GitHub/Compiler-Construction/LanguageSpecs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/CodingProjects/GitHub/Compiler-Construction/LangSpecs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AE6BFE9-4A06-3A46-8032-58FAC3DD292D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{150159C1-C4BA-8C44-A509-D4CCABE6EA7B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23540" activeTab="1" xr2:uid="{3FEBC4A9-0A37-F649-BEF0-00E8881A387D}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" activeTab="1" xr2:uid="{3FEBC4A9-0A37-F649-BEF0-00E8881A387D}"/>
   </bookViews>
   <sheets>
     <sheet name="FirstFollow" sheetId="1" r:id="rId1"/>
@@ -1182,87 +1182,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">FOR BO ID IN </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="17"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;range&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="17"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">BC START </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="17"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;statements&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="17"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">END | WHILE BO </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="17"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;booleanExpr&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="17"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">BC START </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="17"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">&lt;statements&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="17"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">END </t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">LT | LE | GT | GE | EQ | NE </t>
   </si>
   <si>
@@ -1543,13 +1462,94 @@
   </si>
   <si>
     <t>arithmeticOrBooleanExpr</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">FOR BO ID IN </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;range&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="17"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">BC START </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;statements&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="17"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">END | WHILE BO </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;arithmeticOrBooleanExpr&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="17"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">BC START </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="17"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;statements&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="17"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">END </t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1653,13 +1653,25 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="17"/>
+      <color rgb="FFFF0000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="9">
@@ -1774,7 +1786,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1815,6 +1827,18 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1842,6 +1866,21 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1851,31 +1890,10 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2207,11 +2225,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="54" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="16"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="20"/>
     </row>
     <row r="2" spans="1:3" ht="34" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -2265,7 +2283,7 @@
         <v>113</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2276,7 +2294,7 @@
         <v>86</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2353,7 +2371,7 @@
         <v>92</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2364,7 +2382,7 @@
         <v>93</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2383,7 +2401,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>132</v>
@@ -2394,10 +2412,10 @@
         <v>15</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>171</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="62" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2408,7 +2426,7 @@
         <v>42</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="62" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2441,7 +2459,7 @@
         <v>96</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="62" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2452,7 +2470,7 @@
         <v>45</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="62" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2463,7 +2481,7 @@
         <v>98</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="62" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2474,7 +2492,7 @@
         <v>97</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="62" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2485,7 +2503,7 @@
         <v>95</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2507,7 +2525,7 @@
         <v>100</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2544,11 +2562,11 @@
       </c>
     </row>
     <row r="32" spans="1:3" ht="54" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="B32" s="15"/>
-      <c r="C32" s="16"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="20"/>
     </row>
     <row r="33" spans="1:3" ht="34" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
@@ -2566,7 +2584,7 @@
         <v>28</v>
       </c>
       <c r="B34" s="12" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C34" s="6" t="s">
         <v>128</v>
@@ -2574,10 +2592,10 @@
     </row>
     <row r="35" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B35" s="12" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>128</v>
@@ -2585,10 +2603,10 @@
     </row>
     <row r="36" spans="1:3" ht="48" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>128</v>
@@ -2596,7 +2614,7 @@
     </row>
     <row r="37" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B37" s="12" t="s">
         <v>48</v>
@@ -2610,10 +2628,10 @@
         <v>72</v>
       </c>
       <c r="B38" s="12" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2624,7 +2642,7 @@
         <v>47</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="42" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2657,7 +2675,7 @@
         <v>117</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="62" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2668,7 +2686,7 @@
         <v>103</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="62" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2695,13 +2713,13 @@
     </row>
     <row r="46" spans="1:3" ht="42" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B46" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="C46" s="6" t="s">
         <v>191</v>
-      </c>
-      <c r="C46" s="6" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2734,12 +2752,12 @@
         <v>106</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B50" s="5" t="s">
         <v>107</v>
@@ -2756,7 +2774,7 @@
         <v>39</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="62" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2767,7 +2785,7 @@
         <v>108</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2797,7 +2815,7 @@
         <v>35</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C55" s="6" t="s">
         <v>130</v>
@@ -2822,7 +2840,7 @@
         <v>112</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="74" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2837,11 +2855,11 @@
       </c>
     </row>
     <row r="59" spans="1:3" ht="74" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="17" t="s">
-        <v>180</v>
-      </c>
-      <c r="B59" s="18"/>
-      <c r="C59" s="19"/>
+      <c r="A59" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="B59" s="22"/>
+      <c r="C59" s="23"/>
     </row>
     <row r="60" spans="1:3" ht="74" customHeight="1" thickTop="1" x14ac:dyDescent="0.2"/>
     <row r="61" spans="1:3" ht="74" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2901,14 +2919,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AB0AD01-E814-8C4E-B795-59A92B7C67F0}">
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A34" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.83203125" style="3" customWidth="1"/>
     <col min="3" max="3" width="6" style="3" customWidth="1"/>
     <col min="4" max="4" width="146.83203125" style="3" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" style="3" bestFit="1" customWidth="1"/>
@@ -2917,33 +2935,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="85" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="22"/>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="26"/>
     </row>
     <row r="2" spans="1:6" ht="50" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="25"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="34"/>
     </row>
     <row r="3" spans="1:6" ht="54" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="27"/>
+      <c r="C3" s="30"/>
       <c r="D3" s="2" t="s">
         <v>49</v>
       </c>
@@ -2958,7 +2976,7 @@
       <c r="A4" s="4">
         <v>1</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="36" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="9" t="s">
@@ -2967,10 +2985,10 @@
       <c r="D4" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="F4" s="29" t="s">
+      <c r="F4" s="15" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2978,7 +2996,7 @@
       <c r="A5" s="4">
         <v>2</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="36" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="9" t="s">
@@ -2987,10 +3005,10 @@
       <c r="D5" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="F5" s="29" t="s">
+      <c r="F5" s="15" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2998,7 +3016,7 @@
       <c r="A6" s="4">
         <v>3</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="36" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="9" t="s">
@@ -3007,10 +3025,10 @@
       <c r="D6" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="E6" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="F6" s="29" t="s">
+      <c r="F6" s="15" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3018,7 +3036,7 @@
       <c r="A7" s="4">
         <v>4</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="36" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="9" t="s">
@@ -3027,10 +3045,10 @@
       <c r="D7" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="E7" s="28" t="s">
+      <c r="E7" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="F7" s="29" t="s">
+      <c r="F7" s="15" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3038,7 +3056,7 @@
       <c r="A8" s="4">
         <v>5</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="36" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="9" t="s">
@@ -3047,10 +3065,10 @@
       <c r="D8" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="E8" s="30" t="s">
+      <c r="E8" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="F8" s="30" t="s">
+      <c r="F8" s="16" t="s">
         <v>116</v>
       </c>
     </row>
@@ -3058,7 +3076,7 @@
       <c r="A9" s="4">
         <v>6</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="36" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="9" t="s">
@@ -3067,10 +3085,10 @@
       <c r="D9" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="F9" s="29" t="s">
+      <c r="F9" s="15" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3078,7 +3096,7 @@
       <c r="A10" s="4">
         <v>7</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="36" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="9" t="s">
@@ -3087,10 +3105,10 @@
       <c r="D10" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="E10" s="28" t="s">
+      <c r="E10" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="F10" s="29" t="s">
+      <c r="F10" s="15" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3098,7 +3116,7 @@
       <c r="A11" s="4">
         <v>8</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="36" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="9" t="s">
@@ -3107,10 +3125,10 @@
       <c r="D11" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="E11" s="31" t="s">
+      <c r="E11" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="F11" s="31" t="s">
+      <c r="F11" s="27" t="s">
         <v>65</v>
       </c>
     </row>
@@ -3118,7 +3136,7 @@
       <c r="A12" s="4">
         <v>9</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="36" t="s">
         <v>87</v>
       </c>
       <c r="C12" s="9" t="s">
@@ -3127,26 +3145,26 @@
       <c r="D12" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
     </row>
     <row r="13" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>10</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="36" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>50</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="E13" s="31" t="s">
+        <v>169</v>
+      </c>
+      <c r="E13" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="F13" s="31" t="s">
+      <c r="F13" s="27" t="s">
         <v>65</v>
       </c>
     </row>
@@ -3154,7 +3172,7 @@
       <c r="A14" s="4">
         <v>11</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="36" t="s">
         <v>88</v>
       </c>
       <c r="C14" s="9" t="s">
@@ -3163,14 +3181,14 @@
       <c r="D14" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="E14" s="32"/>
-      <c r="F14" s="32"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
     </row>
     <row r="15" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>12</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="36" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="9" t="s">
@@ -3179,10 +3197,10 @@
       <c r="D15" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="E15" s="28" t="s">
+      <c r="E15" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="F15" s="29" t="s">
+      <c r="F15" s="15" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3190,7 +3208,7 @@
       <c r="A16" s="4">
         <v>13</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="36" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="9" t="s">
@@ -3199,10 +3217,10 @@
       <c r="D16" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="E16" s="28" t="s">
+      <c r="E16" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="F16" s="29" t="s">
+      <c r="F16" s="15" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3210,7 +3228,7 @@
       <c r="A17" s="4">
         <v>14</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="36" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="9" t="s">
@@ -3219,10 +3237,10 @@
       <c r="D17" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="E17" s="28" t="s">
+      <c r="E17" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="F17" s="29" t="s">
+      <c r="F17" s="15" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3230,7 +3248,7 @@
       <c r="A18" s="4">
         <v>15</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="B18" s="36" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="9" t="s">
@@ -3239,10 +3257,10 @@
       <c r="D18" s="8" t="s">
         <v>147</v>
       </c>
-      <c r="E18" s="28" t="s">
+      <c r="E18" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="F18" s="29" t="s">
+      <c r="F18" s="15" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3250,19 +3268,19 @@
       <c r="A19" s="4">
         <v>16</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="36" t="s">
         <v>15</v>
       </c>
       <c r="C19" s="9" t="s">
         <v>50</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="E19" s="28" t="s">
+        <v>175</v>
+      </c>
+      <c r="E19" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="F19" s="29" t="s">
+      <c r="F19" s="15" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3270,27 +3288,27 @@
       <c r="A20" s="4">
         <v>17</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="36" t="s">
         <v>16</v>
       </c>
       <c r="C20" s="9" t="s">
         <v>50</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="E20" s="30" t="s">
+        <v>184</v>
+      </c>
+      <c r="E20" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="F20" s="30" t="s">
-        <v>194</v>
+      <c r="F20" s="16" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>18</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="36" t="s">
         <v>18</v>
       </c>
       <c r="C21" s="9" t="s">
@@ -3299,10 +3317,10 @@
       <c r="D21" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="E21" s="28" t="s">
+      <c r="E21" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="F21" s="29" t="s">
+      <c r="F21" s="15" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3310,7 +3328,7 @@
       <c r="A22" s="4">
         <v>19</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="36" t="s">
         <v>19</v>
       </c>
       <c r="C22" s="9" t="s">
@@ -3319,10 +3337,10 @@
       <c r="D22" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="E22" s="28" t="s">
+      <c r="E22" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="F22" s="29" t="s">
+      <c r="F22" s="15" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3330,7 +3348,7 @@
       <c r="A23" s="4">
         <v>20</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="35" t="s">
         <v>20</v>
       </c>
       <c r="C23" s="9" t="s">
@@ -3339,10 +3357,10 @@
       <c r="D23" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="E23" s="28" t="s">
+      <c r="E23" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="F23" s="29" t="s">
+      <c r="F23" s="15" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3350,7 +3368,7 @@
       <c r="A24" s="4">
         <v>21</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="36" t="s">
         <v>21</v>
       </c>
       <c r="C24" s="9" t="s">
@@ -3359,10 +3377,10 @@
       <c r="D24" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="E24" s="28" t="s">
+      <c r="E24" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="F24" s="29" t="s">
+      <c r="F24" s="15" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3370,7 +3388,7 @@
       <c r="A25" s="4">
         <v>22</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="36" t="s">
         <v>22</v>
       </c>
       <c r="C25" s="9" t="s">
@@ -3379,10 +3397,10 @@
       <c r="D25" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="E25" s="28" t="s">
+      <c r="E25" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="F25" s="29" t="s">
+      <c r="F25" s="15" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3390,7 +3408,7 @@
       <c r="A26" s="4">
         <v>23</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="36" t="s">
         <v>23</v>
       </c>
       <c r="C26" s="9" t="s">
@@ -3399,10 +3417,10 @@
       <c r="D26" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="E26" s="28" t="s">
+      <c r="E26" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="F26" s="29" t="s">
+      <c r="F26" s="15" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3410,7 +3428,7 @@
       <c r="A27" s="4">
         <v>24</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="36" t="s">
         <v>24</v>
       </c>
       <c r="C27" s="9" t="s">
@@ -3419,10 +3437,10 @@
       <c r="D27" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="E27" s="28" t="s">
+      <c r="E27" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="F27" s="29" t="s">
+      <c r="F27" s="15" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3430,7 +3448,7 @@
       <c r="A28" s="4">
         <v>25</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="36" t="s">
         <v>25</v>
       </c>
       <c r="C28" s="9" t="s">
@@ -3439,10 +3457,10 @@
       <c r="D28" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="E28" s="28" t="s">
+      <c r="E28" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="F28" s="29" t="s">
+      <c r="F28" s="15" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3450,7 +3468,7 @@
       <c r="A29" s="4">
         <v>26</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="B29" s="36" t="s">
         <v>26</v>
       </c>
       <c r="C29" s="9" t="s">
@@ -3459,31 +3477,31 @@
       <c r="D29" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="E29" s="28" t="s">
+      <c r="E29" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="F29" s="29" t="s">
+      <c r="F29" s="15" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="79" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="20" t="s">
+      <c r="A30" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="B30" s="21"/>
-      <c r="C30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="22"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="26"/>
     </row>
     <row r="31" spans="1:6" ht="54" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B31" s="26" t="s">
+      <c r="B31" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="C31" s="27"/>
+      <c r="C31" s="30"/>
       <c r="D31" s="2" t="s">
         <v>49</v>
       </c>
@@ -3498,7 +3516,7 @@
       <c r="A32" s="4">
         <v>27</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B32" s="36" t="s">
         <v>27</v>
       </c>
       <c r="C32" s="9" t="s">
@@ -3507,10 +3525,10 @@
       <c r="D32" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="E32" s="31" t="s">
+      <c r="E32" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="F32" s="31" t="s">
+      <c r="F32" s="27" t="s">
         <v>65</v>
       </c>
     </row>
@@ -3518,7 +3536,7 @@
       <c r="A33" s="4">
         <v>28</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="B33" s="36" t="s">
         <v>89</v>
       </c>
       <c r="C33" s="9" t="s">
@@ -3527,46 +3545,46 @@
       <c r="D33" s="5" t="s">
         <v>154</v>
       </c>
-      <c r="E33" s="32"/>
-      <c r="F33" s="32"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
     </row>
     <row r="34" spans="1:6" ht="59" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>29</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="36" t="s">
         <v>28</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>50</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>189</v>
-      </c>
-      <c r="E34" s="30" t="s">
+        <v>188</v>
+      </c>
+      <c r="E34" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="F34" s="30" t="s">
-        <v>195</v>
+      <c r="F34" s="16" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>30</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="36" t="s">
+        <v>186</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D35" s="12" t="s">
         <v>187</v>
       </c>
-      <c r="C35" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D35" s="12" t="s">
-        <v>188</v>
-      </c>
-      <c r="E35" s="30" t="s">
+      <c r="E35" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="F35" s="33" t="s">
+      <c r="F35" s="17" t="s">
         <v>116</v>
       </c>
     </row>
@@ -3574,7 +3592,7 @@
       <c r="A36" s="4">
         <v>31</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="B36" s="36" t="s">
         <v>67</v>
       </c>
       <c r="C36" s="9" t="s">
@@ -3583,10 +3601,10 @@
       <c r="D36" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="E36" s="31" t="s">
+      <c r="E36" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="F36" s="31" t="s">
+      <c r="F36" s="27" t="s">
         <v>121</v>
       </c>
     </row>
@@ -3594,7 +3612,7 @@
       <c r="A37" s="4">
         <v>32</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="B37" s="35" t="s">
         <v>68</v>
       </c>
       <c r="C37" s="9" t="s">
@@ -3603,30 +3621,30 @@
       <c r="D37" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="34"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
     </row>
     <row r="38" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>33</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B38" s="36" t="s">
         <v>72</v>
       </c>
       <c r="C38" s="9" t="s">
         <v>50</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>184</v>
-      </c>
-      <c r="E38" s="34"/>
-      <c r="F38" s="34"/>
+        <v>183</v>
+      </c>
+      <c r="E38" s="31"/>
+      <c r="F38" s="31"/>
     </row>
     <row r="39" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>34</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="35" t="s">
         <v>73</v>
       </c>
       <c r="C39" s="9" t="s">
@@ -3635,14 +3653,14 @@
       <c r="D39" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="E39" s="32"/>
-      <c r="F39" s="32"/>
+      <c r="E39" s="28"/>
+      <c r="F39" s="28"/>
     </row>
     <row r="40" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>35</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="B40" s="36" t="s">
         <v>29</v>
       </c>
       <c r="C40" s="9" t="s">
@@ -3651,10 +3669,10 @@
       <c r="D40" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="E40" s="31" t="s">
+      <c r="E40" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="F40" s="31" t="s">
+      <c r="F40" s="27" t="s">
         <v>80</v>
       </c>
     </row>
@@ -3662,7 +3680,7 @@
       <c r="A41" s="4">
         <v>36</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B41" s="36" t="s">
         <v>71</v>
       </c>
       <c r="C41" s="9" t="s">
@@ -3671,14 +3689,14 @@
       <c r="D41" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="E41" s="32"/>
-      <c r="F41" s="32"/>
+      <c r="E41" s="28"/>
+      <c r="F41" s="28"/>
     </row>
     <row r="42" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>37</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="B42" s="36" t="s">
         <v>30</v>
       </c>
       <c r="C42" s="9" t="s">
@@ -3687,10 +3705,10 @@
       <c r="D42" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="E42" s="31" t="s">
+      <c r="E42" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="F42" s="31" t="s">
+      <c r="F42" s="27" t="s">
         <v>65</v>
       </c>
     </row>
@@ -3698,7 +3716,7 @@
       <c r="A43" s="4">
         <v>38</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B43" s="36" t="s">
         <v>74</v>
       </c>
       <c r="C43" s="9" t="s">
@@ -3707,14 +3725,14 @@
       <c r="D43" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="E43" s="32"/>
-      <c r="F43" s="32"/>
+      <c r="E43" s="28"/>
+      <c r="F43" s="28"/>
     </row>
     <row r="44" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>39</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="36" t="s">
         <v>31</v>
       </c>
       <c r="C44" s="9" t="s">
@@ -3723,10 +3741,10 @@
       <c r="D44" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="E44" s="28" t="s">
+      <c r="E44" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="F44" s="29" t="s">
+      <c r="F44" s="15" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3734,19 +3752,19 @@
       <c r="A45" s="4">
         <v>40</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="B45" s="36" t="s">
         <v>17</v>
       </c>
       <c r="C45" s="9" t="s">
         <v>50</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>177</v>
-      </c>
-      <c r="E45" s="30" t="s">
+        <v>176</v>
+      </c>
+      <c r="E45" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="F45" s="30" t="s">
+      <c r="F45" s="16" t="s">
         <v>85</v>
       </c>
     </row>
@@ -3754,27 +3772,27 @@
       <c r="A46" s="4">
         <v>41</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="B46" s="36" t="s">
+        <v>180</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="D46" s="12" t="s">
         <v>181</v>
       </c>
-      <c r="C46" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D46" s="12" t="s">
-        <v>182</v>
-      </c>
-      <c r="E46" s="33" t="s">
+      <c r="E46" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="F46" s="33" t="s">
-        <v>186</v>
+      <c r="F46" s="17" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>42</v>
       </c>
-      <c r="B47" s="7" t="s">
+      <c r="B47" s="36" t="s">
         <v>77</v>
       </c>
       <c r="C47" s="9" t="s">
@@ -3783,10 +3801,10 @@
       <c r="D47" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E47" s="31" t="s">
+      <c r="E47" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="F47" s="31" t="s">
+      <c r="F47" s="27" t="s">
         <v>81</v>
       </c>
     </row>
@@ -3794,7 +3812,7 @@
       <c r="A48" s="4">
         <v>43</v>
       </c>
-      <c r="B48" s="7" t="s">
+      <c r="B48" s="36" t="s">
         <v>76</v>
       </c>
       <c r="C48" s="9" t="s">
@@ -3803,14 +3821,14 @@
       <c r="D48" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="E48" s="32"/>
-      <c r="F48" s="32"/>
+      <c r="E48" s="28"/>
+      <c r="F48" s="28"/>
     </row>
     <row r="49" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>44</v>
       </c>
-      <c r="B49" s="7" t="s">
+      <c r="B49" s="36" t="s">
         <v>32</v>
       </c>
       <c r="C49" s="9" t="s">
@@ -3819,10 +3837,10 @@
       <c r="D49" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="E49" s="28" t="s">
+      <c r="E49" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="F49" s="29" t="s">
+      <c r="F49" s="15" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3830,19 +3848,19 @@
       <c r="A50" s="4">
         <v>45</v>
       </c>
-      <c r="B50" s="7" t="s">
-        <v>175</v>
+      <c r="B50" s="36" t="s">
+        <v>174</v>
       </c>
       <c r="C50" s="9" t="s">
         <v>50</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="E50" s="28" t="s">
+        <v>164</v>
+      </c>
+      <c r="E50" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="F50" s="29" t="s">
+      <c r="F50" s="15" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3850,7 +3868,7 @@
       <c r="A51" s="4">
         <v>46</v>
       </c>
-      <c r="B51" s="7" t="s">
+      <c r="B51" s="36" t="s">
         <v>33</v>
       </c>
       <c r="C51" s="9" t="s">
@@ -3859,10 +3877,10 @@
       <c r="D51" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="E51" s="28" t="s">
+      <c r="E51" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="F51" s="29" t="s">
+      <c r="F51" s="15" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3870,7 +3888,7 @@
       <c r="A52" s="4">
         <v>47</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="B52" s="36" t="s">
         <v>34</v>
       </c>
       <c r="C52" s="9" t="s">
@@ -3879,10 +3897,10 @@
       <c r="D52" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="E52" s="28" t="s">
+      <c r="E52" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="F52" s="29" t="s">
+      <c r="F52" s="15" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3890,7 +3908,7 @@
       <c r="A53" s="4">
         <v>48</v>
       </c>
-      <c r="B53" s="7" t="s">
+      <c r="B53" s="36" t="s">
         <v>82</v>
       </c>
       <c r="C53" s="9" t="s">
@@ -3899,10 +3917,10 @@
       <c r="D53" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="E53" s="31" t="s">
+      <c r="E53" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="F53" s="31" t="s">
+      <c r="F53" s="27" t="s">
         <v>84</v>
       </c>
     </row>
@@ -3910,7 +3928,7 @@
       <c r="A54" s="4">
         <v>49</v>
       </c>
-      <c r="B54" s="7" t="s">
+      <c r="B54" s="36" t="s">
         <v>83</v>
       </c>
       <c r="C54" s="9" t="s">
@@ -3919,26 +3937,26 @@
       <c r="D54" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="E54" s="32"/>
-      <c r="F54" s="32"/>
+      <c r="E54" s="28"/>
+      <c r="F54" s="28"/>
     </row>
     <row r="55" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>50</v>
       </c>
-      <c r="B55" s="7" t="s">
+      <c r="B55" s="35" t="s">
         <v>35</v>
       </c>
       <c r="C55" s="9" t="s">
         <v>50</v>
       </c>
       <c r="D55" s="12" t="s">
-        <v>183</v>
-      </c>
-      <c r="E55" s="28" t="s">
+        <v>182</v>
+      </c>
+      <c r="E55" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="F55" s="29" t="s">
+      <c r="F55" s="15" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3946,7 +3964,7 @@
       <c r="A56" s="4">
         <v>51</v>
       </c>
-      <c r="B56" s="7" t="s">
+      <c r="B56" s="36" t="s">
         <v>36</v>
       </c>
       <c r="C56" s="9" t="s">
@@ -3955,30 +3973,30 @@
       <c r="D56" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="E56" s="28" t="s">
+      <c r="E56" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="F56" s="29" t="s">
+      <c r="F56" s="15" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="48" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>52</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="B57" s="36" t="s">
         <v>37</v>
       </c>
       <c r="C57" s="9" t="s">
         <v>50</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="E57" s="28" t="s">
+        <v>197</v>
+      </c>
+      <c r="E57" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="F57" s="29" t="s">
+      <c r="F57" s="15" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3986,7 +4004,7 @@
       <c r="A58" s="4">
         <v>53</v>
       </c>
-      <c r="B58" s="7" t="s">
+      <c r="B58" s="36" t="s">
         <v>38</v>
       </c>
       <c r="C58" s="9" t="s">
@@ -3995,10 +4013,10 @@
       <c r="D58" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E58" s="28" t="s">
+      <c r="E58" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="F58" s="29" t="s">
+      <c r="F58" s="15" t="s">
         <v>66</v>
       </c>
     </row>
@@ -4051,11 +4069,6 @@
     <row r="100" ht="74" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A30:F30"/>
-    <mergeCell ref="E32:E33"/>
-    <mergeCell ref="F32:F33"/>
-    <mergeCell ref="E42:E43"/>
-    <mergeCell ref="B31:C31"/>
     <mergeCell ref="E53:E54"/>
     <mergeCell ref="F53:F54"/>
     <mergeCell ref="E36:E39"/>
@@ -4072,6 +4085,11 @@
     <mergeCell ref="F11:F12"/>
     <mergeCell ref="E13:E14"/>
     <mergeCell ref="F13:F14"/>
+    <mergeCell ref="A30:F30"/>
+    <mergeCell ref="E32:E33"/>
+    <mergeCell ref="F32:F33"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="B31:C31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="53" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>